<commit_message>
added draft of figure
</commit_message>
<xml_diff>
--- a/4_aviation/modal_share/data/data.xlsx
+++ b/4_aviation/modal_share/data/data.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelweinold/github/phd_publication_figures/4_aviation/modal_share/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A844AB18-6295-1E47-8497-7566EEEFD134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049C1DD6-12C6-EB49-B262-D87B26DEE175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" activeTab="3" xr2:uid="{3D3106B3-D52F-F549-8C18-189FCB3EBB1B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{3D3106B3-D52F-F549-8C18-189FCB3EBB1B}"/>
   </bookViews>
   <sheets>
-    <sheet name="freight" sheetId="1" r:id="rId1"/>
-    <sheet name="Japan" sheetId="2" r:id="rId2"/>
-    <sheet name="EU" sheetId="3" r:id="rId3"/>
-    <sheet name="USA" sheetId="4" r:id="rId4"/>
+    <sheet name="Japan" sheetId="2" r:id="rId1"/>
+    <sheet name="EU" sheetId="3" r:id="rId2"/>
+    <sheet name="USA" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,47 +38,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
-  <si>
-    <t>country</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="35">
   <si>
     <t>year</t>
   </si>
   <si>
-    <t>share of air freight (by value)</t>
-  </si>
-  <si>
-    <t>share of air freight (by volume/weight)</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>world</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.icao.int/sustainability/economic-policy/Pages/Facts-and-Figures.aspx </t>
-  </si>
-  <si>
-    <t>colombia</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>CH</t>
-  </si>
-  <si>
     <t>distance</t>
   </si>
   <si>
-    <t>rail</t>
-  </si>
-  <si>
     <t>car</t>
   </si>
   <si>
@@ -141,6 +110,39 @@
   </si>
   <si>
     <t xml:space="preserve">https://transportgeography.org/contents/chapter5/transportation-modes-modal-competition-modal-shift/modal-split-distance-passenger-united-states/ </t>
+  </si>
+  <si>
+    <t>50-499</t>
+  </si>
+  <si>
+    <t>1000-1499</t>
+  </si>
+  <si>
+    <t>&gt;1500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bts.dot.gov/sites/bts.dot.gov/files/legacy/publications/america_on_the_go/long_distance_transportation_patterns/pdf/entire.pdf </t>
+  </si>
+  <si>
+    <t>distance (air) [miles]</t>
+  </si>
+  <si>
+    <t>air [%]</t>
+  </si>
+  <si>
+    <t>distance (car) [miles]</t>
+  </si>
+  <si>
+    <t>car [%]</t>
+  </si>
+  <si>
+    <t>distance [km]</t>
+  </si>
+  <si>
+    <t>rail [%]</t>
+  </si>
+  <si>
+    <t>other [%]</t>
   </si>
 </sst>
 </file>
@@ -508,146 +510,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5743C5-9AF5-114C-80A1-66736DEAE099}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>2017</v>
-      </c>
-      <c r="C2">
-        <v>34.6</v>
-      </c>
-      <c r="D2">
-        <v>0.5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>2016</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>0.48</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>2016</v>
-      </c>
-      <c r="C4">
-        <v>47.7</v>
-      </c>
-      <c r="D4">
-        <v>0.7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>2020</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{38B7583D-C5B8-2B41-8914-DF8571DE7B3F}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{1D3D33EF-4337-5346-9F0A-F2CE36B0CA1C}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{9C3E3B4A-B21C-7F42-BD95-7BBA61AD12A4}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC3264E-9BD9-EA42-8323-43E4C578A4AD}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>3.2</v>
@@ -663,15 +560,15 @@
         <v>1.2000000000000028</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>10.1</v>
@@ -687,15 +584,15 @@
         <v>2.3000000000000114</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>16.3</v>
@@ -711,15 +608,15 @@
         <v>3.2999999999999972</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>43.7</v>
@@ -735,15 +632,15 @@
         <v>4.3000000000000114</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>69.099999999999994</v>
@@ -759,15 +656,15 @@
         <v>3.2000000000000028</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>45.2</v>
@@ -783,15 +680,15 @@
         <v>3.4000000000000057</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>10.8</v>
@@ -807,15 +704,15 @@
         <v>0.79999999999999716</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>26.730000000000004</v>
@@ -834,12 +731,12 @@
         <v>2005</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>25.42</v>
@@ -858,12 +755,12 @@
         <v>2005</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>41.07</v>
@@ -882,12 +779,12 @@
         <v>2005</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>62.499999999999993</v>
@@ -906,12 +803,12 @@
         <v>2005</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>30.950000000000003</v>
@@ -930,12 +827,12 @@
         <v>2005</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>7.79</v>
@@ -954,7 +851,7 @@
         <v>2005</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -975,40 +872,41 @@
     <hyperlink ref="G14" r:id="rId13" xr:uid="{66DC057A-9C37-964B-B0DA-6CFD642E2772}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7294FF-0B36-3B43-8960-C30E665FB955}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1032,7 +930,7 @@
         <v>2015</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1056,7 +954,7 @@
         <v>2015</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1080,7 +978,7 @@
         <v>2015</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1104,7 +1002,7 @@
         <v>2015</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1128,7 +1026,7 @@
         <v>2015</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1152,7 +1050,7 @@
         <v>2015</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1176,7 +1074,7 @@
         <v>2015</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1200,7 +1098,7 @@
         <v>2015</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1224,7 +1122,7 @@
         <v>2015</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1248,7 +1146,7 @@
         <v>2015</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1268,31 +1166,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE46616-568A-D346-B6B1-8A0E294DFA3E}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1308,8 +1209,11 @@
       <c r="D2">
         <v>95.326050168135495</v>
       </c>
+      <c r="E2">
+        <v>2000</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1325,8 +1229,11 @@
       <c r="D3">
         <v>95.906560665323397</v>
       </c>
+      <c r="E3">
+        <v>2000</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1342,8 +1249,11 @@
       <c r="D4">
         <v>96.039978725801802</v>
       </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1359,8 +1269,11 @@
       <c r="D5">
         <v>96.013011245492294</v>
       </c>
+      <c r="E5">
+        <v>2000</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1376,8 +1289,11 @@
       <c r="D6">
         <v>96.233009111174795</v>
       </c>
+      <c r="E6">
+        <v>2000</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1393,8 +1309,11 @@
       <c r="D7">
         <v>96.478555116097695</v>
       </c>
+      <c r="E7">
+        <v>2000</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1410,8 +1329,11 @@
       <c r="D8">
         <v>96.069784888249103</v>
       </c>
+      <c r="E8">
+        <v>2000</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1427,8 +1349,11 @@
       <c r="D9">
         <v>95.335985555617896</v>
       </c>
+      <c r="E9">
+        <v>2000</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1444,8 +1369,11 @@
       <c r="D10">
         <v>94.3424468073746</v>
       </c>
+      <c r="E10">
+        <v>2000</v>
+      </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1461,8 +1389,11 @@
       <c r="D11">
         <v>92.251757412856904</v>
       </c>
+      <c r="E11">
+        <v>2000</v>
+      </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1478,8 +1409,11 @@
       <c r="D12">
         <v>87.6155290990027</v>
       </c>
+      <c r="E12">
+        <v>2000</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1495,8 +1429,11 @@
       <c r="D13">
         <v>81.189090544186399</v>
       </c>
+      <c r="E13">
+        <v>2000</v>
+      </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1512,8 +1449,11 @@
       <c r="D14">
         <v>73.766105888977805</v>
       </c>
+      <c r="E14">
+        <v>2000</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1529,8 +1469,11 @@
       <c r="D15">
         <v>66.404846877306994</v>
       </c>
+      <c r="E15">
+        <v>2000</v>
+      </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1546,8 +1489,11 @@
       <c r="D16">
         <v>59.112556333414901</v>
       </c>
+      <c r="E16">
+        <v>2000</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1563,8 +1509,11 @@
       <c r="D17">
         <v>52.039709566287797</v>
       </c>
+      <c r="E17">
+        <v>2000</v>
+      </c>
       <c r="F17" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1580,8 +1529,11 @@
       <c r="D18">
         <v>44.023612396790099</v>
       </c>
+      <c r="E18">
+        <v>2000</v>
+      </c>
       <c r="F18" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1597,8 +1549,11 @@
       <c r="D19">
         <v>36.009404432643798</v>
       </c>
+      <c r="E19">
+        <v>2000</v>
+      </c>
       <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1608,8 +1563,11 @@
       <c r="D20">
         <v>28.5440500275426</v>
       </c>
+      <c r="E20">
+        <v>2000</v>
+      </c>
       <c r="F20" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1619,8 +1577,11 @@
       <c r="D21">
         <v>21.000717474699499</v>
       </c>
+      <c r="E21">
+        <v>2000</v>
+      </c>
       <c r="F21" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1630,8 +1591,11 @@
       <c r="D22">
         <v>13.56038917455</v>
       </c>
+      <c r="E22">
+        <v>2000</v>
+      </c>
       <c r="F22" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1641,8 +1605,11 @@
       <c r="D23">
         <v>7.1665183543681898</v>
       </c>
+      <c r="E23">
+        <v>2000</v>
+      </c>
       <c r="F23" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1652,14 +1619,124 @@
       <c r="D24">
         <v>2.1490356224971801</v>
       </c>
+      <c r="E24">
+        <v>2000</v>
+      </c>
       <c r="F24" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32">
+        <v>95.133437990580802</v>
+      </c>
+      <c r="C32">
+        <v>1.72684458398744</v>
+      </c>
+      <c r="D32">
+        <v>2001</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>61.8524332810047</v>
+      </c>
+      <c r="C33">
+        <v>33.751962323390899</v>
+      </c>
+      <c r="D33">
+        <v>2001</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <v>42.229199372056499</v>
+      </c>
+      <c r="C34">
+        <v>54.945054945054899</v>
+      </c>
+      <c r="D34">
+        <v>2001</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35">
+        <v>31.554160125588702</v>
+      </c>
+      <c r="C35">
+        <v>65.463108320251095</v>
+      </c>
+      <c r="D35">
+        <v>2001</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36">
+        <v>14.913657770800601</v>
+      </c>
+      <c r="C36">
+        <v>81.789638932496004</v>
+      </c>
+      <c r="D36">
+        <v>2001</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{70639DC6-E75A-054C-9D9F-F1991040E7FB}"/>
     <hyperlink ref="F3:F24" r:id="rId2" display="https://transportgeography.org/contents/chapter5/transportation-modes-modal-competition-modal-shift/modal-split-distance-passenger-united-states/ " xr:uid="{81847900-F917-204C-A665-127F75DC69DA}"/>
+    <hyperlink ref="E32" r:id="rId3" xr:uid="{432AE11F-A430-E744-98AC-A35B4EFFE5E4}"/>
+    <hyperlink ref="E33" r:id="rId4" xr:uid="{F25BEB94-A813-5042-A75B-AB411E2CCC08}"/>
+    <hyperlink ref="E34" r:id="rId5" xr:uid="{BD1FCC61-024C-EC49-B987-CF60AAA867E4}"/>
+    <hyperlink ref="E36" r:id="rId6" xr:uid="{AB7D5484-B196-3D46-BFDD-DBC95472C366}"/>
+    <hyperlink ref="E35" r:id="rId7" xr:uid="{35C73D1D-4CA2-6646-9C49-A9C00556189F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>